<commit_message>
fixed ema excel sheet, derp
</commit_message>
<xml_diff>
--- a/resources/btc-ema.xlsx
+++ b/resources/btc-ema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC572371-063A-4761-8BE0-A9BEA2084434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E55D67-76C3-48F4-B5B7-23EDBBEA8FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28575" yWindow="4575" windowWidth="16410" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28590" yWindow="-8955" windowWidth="16410" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -370,7 +370,7 @@
   <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,8 +543,8 @@
         <v>13311</v>
       </c>
       <c r="C15">
-        <f>AVERAGE(B2:B15)</f>
-        <v>13310.4</v>
+        <f>((B15-C14)*(2/15))+C14</f>
+        <v>13310.975238095238</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,8 +555,8 @@
         <v>13322.1</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C15:C78" si="0">AVERAGE(B3:B16)</f>
-        <v>13310.621428571427</v>
+        <f t="shared" ref="C16:C79" si="0">((B16-C15)*(2/15))+C15</f>
+        <v>13312.458539682539</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>13308.899999999998</v>
+        <v>13313.744067724867</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>13307.735714285713</v>
+        <v>13315.911525361551</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>13303.864285714286</v>
+        <v>13312.736655313343</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>13305.17142857143</v>
+        <v>13309.985101271564</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>13306.407142857146</v>
+        <v>13307.600421102023</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>13307.607142857145</v>
+        <v>13299.493698288419</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>13301.714285714286</v>
+        <v>13290.147871849964</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>13297.714285714286</v>
+        <v>13280.581488936636</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>13289.464285714286</v>
+        <v>13267.023957078418</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>13277.364285714284</v>
+        <v>13255.260762801296</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>13264.5</v>
+        <v>13243.612661094456</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>13255.264285714284</v>
+        <v>13236.730972948528</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>13250.678571428569</v>
+        <v>13238.073509888723</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>13247.592857142854</v>
+        <v>13243.51704190356</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>13245.942857142854</v>
+        <v>13250.914769649753</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>13247.921428571428</v>
+        <v>13265.152800363119</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>13257.649999999998</v>
+        <v>13286.905760314703</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>13268.014285714287</v>
+        <v>13306.944992272744</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>13278.378571428573</v>
+        <v>13324.312326636378</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>13294.300000000001</v>
+        <v>13343.697349751528</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>13311.342857142858</v>
+        <v>13360.271036451324</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>13330.178571428574</v>
+        <v>13376.514898257814</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>13351.835714285715</v>
+        <v>13390.592911823438</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>13374.285714285716</v>
+        <v>13404.260523580313</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>13399.114285714286</v>
+        <v>13419.092453769605</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>13422.364285714286</v>
+        <v>13432.213459933657</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>13441.100000000002</v>
+        <v>13442.46499860917</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>13452.335714285715</v>
+        <v>13441.629665461282</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>13462.842857142861</v>
+        <v>13442.225710066445</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>13468.342857142861</v>
+        <v>13441.222282057586</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,7 +928,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>13470.028571428575</v>
+        <v>13442.645977783241</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>13471.907142857146</v>
+        <v>13445.426514078808</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>13474.5</v>
+        <v>13449.169645534967</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,7 +964,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>13475.742857142857</v>
+        <v>13454.227026130304</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>13477.307142857144</v>
+        <v>13458.983422646263</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,7 +988,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>13482.857142857143</v>
+        <v>13472.425632960094</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>13489.742857142855</v>
+        <v>13486.568881898747</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>13495.707142857142</v>
+        <v>13498.573030978914</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>13501.021428571428</v>
+        <v>13510.749960181725</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>13506.642857142857</v>
+        <v>13522.143298824161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>13511.964285714288</v>
+        <v>13530.337525647607</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>13522.95</v>
+        <v>13538.292522227926</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>13537.871428571429</v>
+        <v>13553.853519264203</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>13556.885714285714</v>
+        <v>13573.459716695643</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>13577.571428571429</v>
+        <v>13595.865087802891</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>13592.235714285713</v>
+        <v>13605.589742762506</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>13608.692857142856</v>
+        <v>13618.697777060839</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>13626.864285714284</v>
+        <v>13635.071406786061</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>13641.449999999999</v>
+        <v>13642.941885881253</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>13648.192857142858</v>
+        <v>13644.442967763753</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C67">
         <f t="shared" si="0"/>
-        <v>13654.614285714286</v>
+        <v>13647.637238728586</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="C68">
         <f t="shared" si="0"/>
-        <v>13660.65</v>
+        <v>13649.432273564775</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="C69">
         <f t="shared" si="0"/>
-        <v>13664.114285714286</v>
+        <v>13647.961303756138</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="C70">
         <f t="shared" si="0"/>
-        <v>13668.671428571428</v>
+        <v>13649.56646325532</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="C71">
         <f t="shared" si="0"/>
-        <v>13674.535714285714</v>
+        <v>13651.717601487944</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C72">
         <f t="shared" si="0"/>
-        <v>13682.207142857142</v>
+        <v>13657.808587956219</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="C73">
         <f t="shared" si="0"/>
-        <v>13685.235714285716</v>
+        <v>13663.08744289539</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="C74">
         <f t="shared" si="0"/>
-        <v>13680.678571428571</v>
+        <v>13659.622450509338</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="C75">
         <f t="shared" si="0"/>
-        <v>13673.157142857144</v>
+        <v>13656.499457108093</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="C76">
         <f t="shared" si="0"/>
-        <v>13672.107142857143</v>
+        <v>13656.17952949368</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="C77">
         <f t="shared" si="0"/>
-        <v>13667.27142857143</v>
+        <v>13653.515592227855</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C78">
         <f t="shared" si="0"/>
-        <v>13661.707142857145</v>
+        <v>13654.860179930809</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1311,8 +1311,8 @@
         <v>13639.5</v>
       </c>
       <c r="C79">
-        <f t="shared" ref="C79:C142" si="1">AVERAGE(B66:B79)</f>
-        <v>13657.807142857144</v>
+        <f t="shared" si="0"/>
+        <v>13652.812155940035</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,8 +1323,8 @@
         <v>13671.3</v>
       </c>
       <c r="C80">
-        <f t="shared" si="1"/>
-        <v>13659.028571428571</v>
+        <f t="shared" ref="C80:C143" si="1">((B80-C79)*(2/15))+C79</f>
+        <v>13655.277201814697</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
-        <v>13657.035714285714</v>
+        <v>13653.306908239405</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
-        <v>13656.6</v>
+        <v>13653.532653807484</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
-        <v>13660.214285714286</v>
+        <v>13658.26163329982</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
-        <v>13662.285714285714</v>
+        <v>13662.360082193178</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
-        <v>13665.142857142859</v>
+        <v>13668.138737900754</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="C86">
         <f t="shared" si="1"/>
-        <v>13667.071428571431</v>
+        <v>13675.640239513987</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C87">
         <f t="shared" si="1"/>
-        <v>13670.15</v>
+        <v>13684.288207578789</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="C88">
         <f t="shared" si="1"/>
-        <v>13677.785714285716</v>
+        <v>13692.249779901618</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C89">
         <f t="shared" si="1"/>
-        <v>13685.957142857142</v>
+        <v>13700.02980924807</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="C90">
         <f t="shared" si="1"/>
-        <v>13691.7</v>
+        <v>13704.625834681661</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="C91">
         <f t="shared" si="1"/>
-        <v>13699.35</v>
+        <v>13709.78239005744</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="C92">
         <f t="shared" si="1"/>
-        <v>13705.564285714285</v>
+        <v>13715.224738049781</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="C93">
         <f t="shared" si="1"/>
-        <v>13711.628571428571</v>
+        <v>13716.44810630981</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="C94">
         <f t="shared" si="1"/>
-        <v>13714.128571428571</v>
+        <v>13715.095025468501</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="C95">
         <f t="shared" si="1"/>
-        <v>13721.371428571427</v>
+        <v>13718.669022072701</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="C96">
         <f t="shared" si="1"/>
-        <v>13728.707142857142</v>
+        <v>13723.873152463008</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C97">
         <f t="shared" si="1"/>
-        <v>13734.985714285716</v>
+        <v>13730.943398801273</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="C98">
         <f t="shared" si="1"/>
-        <v>13747</v>
+        <v>13747.777612294438</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="C99">
         <f t="shared" si="1"/>
-        <v>13756.535714285716</v>
+        <v>13759.967263988512</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C100">
         <f t="shared" si="1"/>
-        <v>13765.15</v>
+        <v>13771.304962123377</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C101">
         <f t="shared" si="1"/>
-        <v>13770.935714285715</v>
+        <v>13777.997633840259</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C102">
         <f t="shared" si="1"/>
-        <v>13777.842857142858</v>
+        <v>13786.357949328225</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C103">
         <f t="shared" si="1"/>
-        <v>13785.17142857143</v>
+        <v>13795.270222751129</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
       </c>
       <c r="C104">
         <f t="shared" si="1"/>
-        <v>13795.578571428574</v>
+        <v>13806.594193050978</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="C105">
         <f t="shared" si="1"/>
-        <v>13805.235714285718</v>
+        <v>13816.181633977514</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C106">
         <f t="shared" si="1"/>
-        <v>13812.678571428571</v>
+        <v>13821.330749447179</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C107">
         <f t="shared" si="1"/>
-        <v>13821.335714285715</v>
+        <v>13824.566649520888</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="C108">
         <f t="shared" si="1"/>
-        <v>13828.47857142857</v>
+        <v>13822.131096251436</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="C109">
         <f t="shared" si="1"/>
-        <v>13833.271428571426</v>
+        <v>13820.380283417911</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="C110">
         <f t="shared" si="1"/>
-        <v>13838.949999999999</v>
+        <v>13822.622912295523</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="C111">
         <f t="shared" si="1"/>
-        <v>13842.135714285714</v>
+        <v>13822.473190656119</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="C112">
         <f t="shared" si="1"/>
-        <v>13838.464285714286</v>
+        <v>13820.250098568637</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C113">
         <f t="shared" si="1"/>
-        <v>13840.214285714286</v>
+        <v>13826.043418759486</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C114">
         <f t="shared" si="1"/>
-        <v>13841.135714285716</v>
+        <v>13830.290962924888</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="C115">
         <f t="shared" si="1"/>
-        <v>13842.857142857143</v>
+        <v>13832.332167868237</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="C116">
         <f t="shared" si="1"/>
-        <v>13843.664285714287</v>
+        <v>13834.954545485805</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="C117">
         <f t="shared" si="1"/>
-        <v>13840.835714285715</v>
+        <v>13832.107272754365</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="C118">
         <f t="shared" si="1"/>
-        <v>13837.442857142858</v>
+        <v>13832.186303053782</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="C119">
         <f t="shared" si="1"/>
-        <v>13832.67142857143</v>
+        <v>13829.454795979946</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="C120">
         <f t="shared" si="1"/>
-        <v>13829.607142857145</v>
+        <v>13827.114156515952</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C121">
         <f t="shared" si="1"/>
-        <v>13829.535714285716</v>
+        <v>13829.445602313825</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="C122">
         <f t="shared" si="1"/>
-        <v>13830.992857142859</v>
+        <v>13829.079522005315</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="C123">
         <f t="shared" si="1"/>
-        <v>13831.550000000001</v>
+        <v>13827.442252404606</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="C124">
         <f t="shared" si="1"/>
-        <v>13828.321428571429</v>
+        <v>13822.716618750659</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="C125">
         <f t="shared" si="1"/>
-        <v>13823.385714285714</v>
+        <v>13813.341069583905</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="C126">
         <f t="shared" si="1"/>
-        <v>13819.45714285714</v>
+        <v>13805.002260306052</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="C127">
         <f t="shared" si="1"/>
-        <v>13813.192857142856</v>
+        <v>13801.135292265244</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="C128">
         <f t="shared" si="1"/>
-        <v>13806.257142857139</v>
+        <v>13795.757253296544</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="C129">
         <f t="shared" si="1"/>
-        <v>13799.542857142855</v>
+        <v>13789.869619523672</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="C130">
         <f t="shared" si="1"/>
-        <v>13789.157142857142</v>
+        <v>13778.767003587182</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C131">
         <f t="shared" si="1"/>
-        <v>13781.514285714287</v>
+        <v>13769.144736442224</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="C132">
         <f t="shared" si="1"/>
-        <v>13773.071428571429</v>
+        <v>13761.85877158326</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="C133">
         <f t="shared" si="1"/>
-        <v>13769.17142857143</v>
+        <v>13761.224268705491</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="C134">
         <f t="shared" si="1"/>
-        <v>13765.871428571432</v>
+        <v>13761.821032878093</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="C135">
         <f t="shared" si="1"/>
-        <v>13759.621428571432</v>
+        <v>13761.191561827682</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="C136">
         <f t="shared" si="1"/>
-        <v>13753.392857142861</v>
+        <v>13758.299353583991</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="C137">
         <f t="shared" si="1"/>
-        <v>13747.892857142859</v>
+        <v>13755.832773106125</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="C138">
         <f t="shared" si="1"/>
-        <v>13741.235714285716</v>
+        <v>13748.228403358642</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="C139">
         <f t="shared" si="1"/>
-        <v>13735.528571428571</v>
+        <v>13738.131282910823</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="C140">
         <f t="shared" si="1"/>
-        <v>13729.82857142857</v>
+        <v>13729.18044518938</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="C141">
         <f t="shared" si="1"/>
-        <v>13724.728571428572</v>
+        <v>13725.903052497462</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="C142">
         <f t="shared" si="1"/>
-        <v>13722.357142857145</v>
+        <v>13726.129312164467</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2079,8 +2079,8 @@
         <v>13693.3</v>
       </c>
       <c r="C143">
-        <f t="shared" ref="C143:C200" si="2">AVERAGE(B130:B143)</f>
-        <v>13718.192857142858</v>
+        <f t="shared" si="1"/>
+        <v>13721.752070542538</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2091,8 +2091,8 @@
         <v>13673.1</v>
       </c>
       <c r="C144">
-        <f t="shared" si="2"/>
-        <v>13715.800000000001</v>
+        <f t="shared" ref="C144:C200" si="2">((B144-C143)*(2/15))+C143</f>
+        <v>13715.265127803532</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="C145">
         <f t="shared" si="2"/>
-        <v>13715</v>
+        <v>13712.616444096395</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C146">
         <f t="shared" si="2"/>
-        <v>13717.357142857143</v>
+        <v>13717.267584883542</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="C147">
         <f t="shared" si="2"/>
-        <v>13713.400000000003</v>
+        <v>13715.19190689907</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="C148">
         <f t="shared" si="2"/>
-        <v>13710.571428571431</v>
+        <v>13716.646319312527</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
       </c>
       <c r="C149">
         <f t="shared" si="2"/>
-        <v>13709.878571428575</v>
+        <v>13720.746810070857</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="C150">
         <f t="shared" si="2"/>
-        <v>13708.721428571429</v>
+        <v>13721.087235394743</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="C151">
         <f t="shared" si="2"/>
-        <v>13711.707142857142</v>
+        <v>13729.155604008778</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C152">
         <f t="shared" si="2"/>
-        <v>13718.714285714284</v>
+        <v>13738.188190140942</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="C153">
         <f t="shared" si="2"/>
-        <v>13727.6</v>
+        <v>13746.016431455482</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="C154">
         <f t="shared" si="2"/>
-        <v>13735.621428571427</v>
+        <v>13750.987573928085</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
       </c>
       <c r="C155">
         <f t="shared" si="2"/>
-        <v>13737.264285714284</v>
+        <v>13747.869230737673</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="C156">
         <f t="shared" si="2"/>
-        <v>13738.085714285715</v>
+        <v>13746.69999997265</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="C157">
         <f t="shared" si="2"/>
-        <v>13740.021428571428</v>
+        <v>13743.193333309629</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="C158">
         <f t="shared" si="2"/>
-        <v>13742.978571428572</v>
+        <v>13739.367555535013</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="C159">
         <f t="shared" si="2"/>
-        <v>13743.042857142855</v>
+        <v>13733.625214797012</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="C160">
         <f t="shared" si="2"/>
-        <v>13743.014285714284</v>
+        <v>13735.421852824076</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="C161">
         <f t="shared" si="2"/>
-        <v>13748.385714285714</v>
+        <v>13740.952272447532</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="C162">
         <f t="shared" si="2"/>
-        <v>13752.5</v>
+        <v>13746.651969454528</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="C163">
         <f t="shared" si="2"/>
-        <v>13753.621428571429</v>
+        <v>13748.845040193924</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="C164">
         <f t="shared" si="2"/>
-        <v>13755.964285714288</v>
+        <v>13749.812368168068</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C165">
         <f t="shared" si="2"/>
-        <v>13752.971428571431</v>
+        <v>13748.464052412326</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="C166">
         <f t="shared" si="2"/>
-        <v>13749.42142857143</v>
+        <v>13748.295512090683</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="C167">
         <f t="shared" si="2"/>
-        <v>13747.27142857143</v>
+        <v>13750.762777145259</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="C168">
         <f t="shared" si="2"/>
-        <v>13747.335714285715</v>
+        <v>13755.22107352589</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="C169">
         <f t="shared" si="2"/>
-        <v>13751.492857142859</v>
+        <v>13759.298263722438</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="C170">
         <f t="shared" si="2"/>
-        <v>13755.435714285713</v>
+        <v>13763.96516189278</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C171">
         <f t="shared" si="2"/>
-        <v>13759.899999999998</v>
+        <v>13766.489806973743</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="C172">
         <f t="shared" si="2"/>
-        <v>13763.635714285712</v>
+        <v>13766.531166043911</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="C173">
         <f t="shared" si="2"/>
-        <v>13770.392857142853</v>
+        <v>13769.780343904722</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="C174">
         <f t="shared" si="2"/>
-        <v>13773.521428571426</v>
+        <v>13772.596298050759</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="C175">
         <f t="shared" si="2"/>
-        <v>13774.557142857142</v>
+        <v>13775.103458310658</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="C176">
         <f t="shared" si="2"/>
-        <v>13776.678571428569</v>
+        <v>13780.209663869236</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="C177">
         <f t="shared" si="2"/>
-        <v>13780.271428571428</v>
+        <v>13784.635042020005</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="C178">
         <f t="shared" si="2"/>
-        <v>13784.371428571427</v>
+        <v>13788.483703084004</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="C179">
         <f t="shared" si="2"/>
-        <v>13789.164285714283</v>
+        <v>13790.925876006137</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="C180">
         <f t="shared" si="2"/>
-        <v>13797.764285714284</v>
+        <v>13801.149092538652</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="C181">
         <f t="shared" si="2"/>
-        <v>13802.985714285711</v>
+        <v>13806.315880200165</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="C182">
         <f t="shared" si="2"/>
-        <v>13806.249999999998</v>
+        <v>13809.460429506809</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="C183">
         <f t="shared" si="2"/>
-        <v>13808.464285714284</v>
+        <v>13810.439038905901</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="C184">
         <f t="shared" si="2"/>
-        <v>13808.399999999996</v>
+        <v>13808.167167051781</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="C185">
         <f t="shared" si="2"/>
-        <v>13806.47857142857</v>
+        <v>13801.211544778211</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="C186">
         <f t="shared" si="2"/>
-        <v>13802.442857142856</v>
+        <v>13789.090005474449</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="C187">
         <f t="shared" si="2"/>
-        <v>13795.22857142857</v>
+        <v>13775.864671411189</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="C188">
         <f t="shared" si="2"/>
-        <v>13791.149999999998</v>
+        <v>13770.256048556364</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="C189">
         <f t="shared" si="2"/>
-        <v>13786.557142857142</v>
+        <v>13764.501908748849</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -2644,7 +2644,7 @@
       </c>
       <c r="C190">
         <f t="shared" si="2"/>
-        <v>13777.278571428569</v>
+        <v>13753.701654249002</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="C191">
         <f t="shared" si="2"/>
-        <v>13770.721428571429</v>
+        <v>13749.421433682468</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="C192">
         <f t="shared" si="2"/>
-        <v>13764.1</v>
+        <v>13745.605242524805</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="C193">
         <f t="shared" si="2"/>
-        <v>13758.585714285713</v>
+        <v>13743.471210188165</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="C194">
         <f t="shared" si="2"/>
-        <v>13748.721428571429</v>
+        <v>13741.608382163076</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="C195">
         <f t="shared" si="2"/>
-        <v>13740.964285714284</v>
+        <v>13740.233931208</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C196">
         <f t="shared" si="2"/>
-        <v>13736.714285714286</v>
+        <v>13744.256073713601</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="C197">
         <f t="shared" si="2"/>
-        <v>13733.407142857142</v>
+        <v>13747.755263885121</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="C198">
         <f t="shared" si="2"/>
-        <v>13728.728571428572</v>
+        <v>13745.107895367106</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="C199">
         <f t="shared" si="2"/>
-        <v>13725.092857142858</v>
+        <v>13739.773509318158</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2764,10 +2764,13 @@
       </c>
       <c r="C200">
         <f t="shared" si="2"/>
-        <v>13729.392857142857</v>
+        <v>13743.870374742404</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="C14" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>